<commit_message>
Update for 2015 rankings
</commit_message>
<xml_diff>
--- a/lib/tasks/te.xlsx
+++ b/lib/tasks/te.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="131">
   <si>
     <t>Rank</t>
   </si>
@@ -80,229 +80,331 @@
     <t>XP%</t>
   </si>
   <si>
-    <t>Funchess</t>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jonnu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida International                             </t>
+  </si>
+  <si>
+    <t>TE</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Stephen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California                                        </t>
+  </si>
+  <si>
+    <t>Hodges</t>
+  </si>
+  <si>
+    <t>Bucky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virginia Tech                                     </t>
+  </si>
+  <si>
+    <t>Mills</t>
+  </si>
+  <si>
+    <t>Rodney</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Massachusetts                                     </t>
+  </si>
+  <si>
+    <t>Engram</t>
+  </si>
+  <si>
+    <t>Evan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mississippi                                       </t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Hunter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkansas                                          </t>
+  </si>
+  <si>
+    <t>Serigne</t>
+  </si>
+  <si>
+    <t>Cam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wake Forest                                       </t>
+  </si>
+  <si>
+    <t>Scheu</t>
+  </si>
+  <si>
+    <t>Steven</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vanderbilt                                        </t>
+  </si>
+  <si>
+    <t>Grinnage</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t xml:space="preserve">North Carolina State                              </t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Joel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia State                                     </t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>OJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alabama                                           </t>
+  </si>
+  <si>
+    <t>Watson</t>
+  </si>
+  <si>
+    <t>Deon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Idaho                                             </t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Memphis                                           </t>
+  </si>
+  <si>
+    <t>Adams</t>
+  </si>
+  <si>
+    <t>Jerell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Carolina                                    </t>
+  </si>
+  <si>
+    <t>Gaines</t>
+  </si>
+  <si>
+    <t>Jeremiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMU                                               </t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">South Florida                                     </t>
+  </si>
+  <si>
+    <t>Hooper</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stanford                                          </t>
+  </si>
+  <si>
+    <t>Weiser</t>
+  </si>
+  <si>
+    <t>Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buffalo                                           </t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tulane                                            </t>
+  </si>
+  <si>
+    <t>Kohl</t>
+  </si>
+  <si>
+    <t>Kody</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arizona State                                     </t>
+  </si>
+  <si>
+    <t>Blazevich</t>
+  </si>
+  <si>
+    <t>Jeb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Georgia                                           </t>
+  </si>
+  <si>
+    <t>Dobard</t>
+  </si>
+  <si>
+    <t>Standish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miami                                             </t>
+  </si>
+  <si>
+    <t>Josiah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan State                                    </t>
+  </si>
+  <si>
+    <t>Duzey</t>
+  </si>
+  <si>
+    <t>Jake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iowa                                              </t>
+  </si>
+  <si>
+    <t>Deaver</t>
+  </si>
+  <si>
+    <t>Braxton</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duke                                              </t>
+  </si>
+  <si>
+    <t>McCord</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Michigan                                  </t>
+  </si>
+  <si>
+    <t>Vannett</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ohio State                                        </t>
+  </si>
+  <si>
+    <t>Butt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michigan                                          </t>
+  </si>
+  <si>
+    <t>Griswold</t>
+  </si>
+  <si>
+    <t>Darion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkansas State                                    </t>
+  </si>
+  <si>
+    <t>Roh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boise State                                       </t>
+  </si>
+  <si>
+    <t>Cartwright</t>
+  </si>
+  <si>
+    <t>Kivon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colorado State                                    </t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Griffin</t>
+  </si>
+  <si>
+    <t>Garrett</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Air Force                                         </t>
+  </si>
+  <si>
+    <t>Saunders</t>
+  </si>
+  <si>
+    <t>Mavin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida State                                     </t>
+  </si>
+  <si>
+    <t>Frohnapfel</t>
+  </si>
+  <si>
+    <t>Eric</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marshall                                          </t>
+  </si>
+  <si>
+    <t>Whitney</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Texas Tech                                        </t>
+  </si>
+  <si>
+    <t>Scott</t>
   </si>
   <si>
     <t>Devin</t>
   </si>
   <si>
-    <t xml:space="preserve">Michigan                                          </t>
-  </si>
-  <si>
-    <t>TE</t>
-  </si>
-  <si>
-    <t>Cartwright</t>
-  </si>
-  <si>
-    <t>Kivon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Colorado State                                    </t>
-  </si>
-  <si>
-    <t>O'Leary</t>
-  </si>
-  <si>
-    <t>Nick</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Florida State                                     </t>
-  </si>
-  <si>
-    <t>Engram</t>
-  </si>
-  <si>
-    <t>Evan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mississippi                                       </t>
-  </si>
-  <si>
-    <t>Kroft</t>
-  </si>
-  <si>
-    <t>Tyler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rutgers                                           </t>
-  </si>
-  <si>
-    <t>Hamlett</t>
-  </si>
-  <si>
-    <t>Connor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oregon State                                      </t>
-  </si>
-  <si>
-    <t>Russell</t>
-  </si>
-  <si>
-    <t>Tyreese</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eastern Michigan                                  </t>
-  </si>
-  <si>
-    <t>Henry</t>
-  </si>
-  <si>
-    <t>Hunter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arkansas                                          </t>
-  </si>
-  <si>
-    <t>Mundt</t>
-  </si>
-  <si>
-    <t>Johnny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oregon                                            </t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Caleb</t>
-  </si>
-  <si>
-    <t>Koyack</t>
-  </si>
-  <si>
-    <t>Ben</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notre Dame                                        </t>
-  </si>
-  <si>
-    <t>Griswold</t>
-  </si>
-  <si>
-    <t>Darion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arkansas State                                    </t>
-  </si>
-  <si>
-    <t>Williams</t>
-  </si>
-  <si>
-    <t>Maxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minnesota                                         </t>
-  </si>
-  <si>
-    <t>James</t>
-  </si>
-  <si>
-    <t>Jesse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Penn State                                        </t>
-  </si>
-  <si>
-    <t>Heuerman</t>
-  </si>
-  <si>
-    <t>Jeff</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ohio State                                        </t>
-  </si>
-  <si>
-    <t>Saxton</t>
-  </si>
-  <si>
-    <t>Wes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Alabama                                     </t>
-  </si>
-  <si>
-    <t>Freeman</t>
-  </si>
-  <si>
-    <t>Billy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Jose State                                    </t>
-  </si>
-  <si>
-    <t>Howard</t>
-  </si>
-  <si>
-    <t>O.J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alabama                                           </t>
-  </si>
-  <si>
-    <t>Pierce</t>
-  </si>
-  <si>
-    <t>Casey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kent                                              </t>
-  </si>
-  <si>
-    <t>Christian</t>
-  </si>
-  <si>
-    <t>Gerald</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louisville                                        </t>
-  </si>
-  <si>
-    <t>Garner</t>
-  </si>
-  <si>
-    <t>Manasseh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pittsburgh                                        </t>
-  </si>
-  <si>
-    <t>Walford</t>
-  </si>
-  <si>
-    <t>Clive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miami                                             </t>
-  </si>
-  <si>
-    <t>Carter</t>
-  </si>
-  <si>
-    <t>Kyle</t>
-  </si>
-  <si>
-    <t>Baylis</t>
-  </si>
-  <si>
-    <t>Nelson</t>
-  </si>
-  <si>
-    <t>De'Marieya</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arizona State                                     </t>
-  </si>
-  <si>
-    <t>Deaver</t>
-  </si>
-  <si>
-    <t>Braxton</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duke                                              </t>
+    <t xml:space="preserve">Western Kentucky                                  </t>
+  </si>
+  <si>
+    <t>McGee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida                                           </t>
   </si>
 </sst>
 </file>
@@ -311,10 +413,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="#,##0.0000000"/>
-    <numFmt numFmtId="60" formatCode="#,##0.0"/>
+    <numFmt numFmtId="59" formatCode="#,##0.0"/>
+    <numFmt numFmtId="60" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -326,17 +428,12 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="13"/>
       <color indexed="8"/>
       <name val="Verdana"/>
     </font>
@@ -383,24 +480,24 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="60" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1652,7 +1749,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V27"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1768,10 +1865,10 @@
         <v>25</v>
       </c>
       <c r="F2" s="3">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="G2" s="4">
-        <v>14.1666666</v>
+        <v>9.5</v>
       </c>
       <c r="H2" s="3">
         <v>12</v>
@@ -1783,7 +1880,7 @@
         <v>0</v>
       </c>
       <c r="K2" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L2" s="3">
         <v>0</v>
@@ -1792,10 +1889,10 @@
         <v>0</v>
       </c>
       <c r="N2" s="3">
-        <v>986</v>
+        <v>667</v>
       </c>
       <c r="O2" s="3">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="P2" s="3">
         <v>0</v>
@@ -1836,10 +1933,10 @@
         <v>25</v>
       </c>
       <c r="F3" s="3">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G3" s="6">
-        <v>9.5</v>
+        <v>9.3333333</v>
       </c>
       <c r="H3" s="3">
         <v>12</v>
@@ -1851,7 +1948,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L3" s="3">
         <v>0</v>
@@ -1860,10 +1957,10 @@
         <v>0</v>
       </c>
       <c r="N3" s="3">
-        <v>722</v>
+        <v>767</v>
       </c>
       <c r="O3" s="3">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="P3" s="3">
         <v>0</v>
@@ -1904,10 +2001,10 @@
         <v>25</v>
       </c>
       <c r="F4" s="3">
-        <v>111</v>
-      </c>
-      <c r="G4" s="7">
-        <v>9.25</v>
+        <v>103</v>
+      </c>
+      <c r="G4" s="6">
+        <v>8.5833333</v>
       </c>
       <c r="H4" s="3">
         <v>12</v>
@@ -1919,19 +2016,19 @@
         <v>0</v>
       </c>
       <c r="K4" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L4" s="3">
         <v>0</v>
       </c>
       <c r="M4" s="3">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="N4" s="3">
-        <v>630</v>
+        <v>535</v>
       </c>
       <c r="O4" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -1972,10 +2069,10 @@
         <v>25</v>
       </c>
       <c r="F5" s="3">
-        <v>103</v>
-      </c>
-      <c r="G5" s="4">
-        <v>8.5833333</v>
+        <v>99</v>
+      </c>
+      <c r="G5" s="7">
+        <v>8.25</v>
       </c>
       <c r="H5" s="3">
         <v>12</v>
@@ -1987,7 +2084,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L5" s="3">
         <v>0</v>
@@ -1996,10 +2093,10 @@
         <v>0</v>
       </c>
       <c r="N5" s="3">
-        <v>616</v>
+        <v>636</v>
       </c>
       <c r="O5" s="3">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -2040,10 +2137,10 @@
         <v>25</v>
       </c>
       <c r="F6" s="3">
-        <v>100</v>
-      </c>
-      <c r="G6" s="4">
-        <v>8.3333333</v>
+        <v>93</v>
+      </c>
+      <c r="G6" s="7">
+        <v>7.75</v>
       </c>
       <c r="H6" s="3">
         <v>12</v>
@@ -2064,10 +2161,10 @@
         <v>0</v>
       </c>
       <c r="N6" s="3">
-        <v>701</v>
+        <v>638</v>
       </c>
       <c r="O6" s="3">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="P6" s="3">
         <v>0</v>
@@ -2108,10 +2205,10 @@
         <v>25</v>
       </c>
       <c r="F7" s="3">
-        <v>97</v>
-      </c>
-      <c r="G7" s="4">
-        <v>8.0833333</v>
+        <v>89</v>
+      </c>
+      <c r="G7" s="6">
+        <v>7.4166666</v>
       </c>
       <c r="H7" s="3">
         <v>12</v>
@@ -2123,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L7" s="3">
         <v>0</v>
@@ -2132,10 +2229,10 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>617</v>
+        <v>599</v>
       </c>
       <c r="O7" s="3">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="P7" s="3">
         <v>0</v>
@@ -2176,10 +2273,10 @@
         <v>25</v>
       </c>
       <c r="F8" s="3">
-        <v>96</v>
-      </c>
-      <c r="G8" s="3">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="G8" s="6">
+        <v>7.1666666</v>
       </c>
       <c r="H8" s="3">
         <v>12</v>
@@ -2200,10 +2297,10 @@
         <v>0</v>
       </c>
       <c r="N8" s="3">
-        <v>664</v>
+        <v>566</v>
       </c>
       <c r="O8" s="3">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="P8" s="3">
         <v>0</v>
@@ -2244,10 +2341,10 @@
         <v>25</v>
       </c>
       <c r="F9" s="3">
-        <v>96</v>
-      </c>
-      <c r="G9" s="3">
-        <v>8</v>
+        <v>86</v>
+      </c>
+      <c r="G9" s="6">
+        <v>7.1666666</v>
       </c>
       <c r="H9" s="3">
         <v>12</v>
@@ -2259,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L9" s="3">
         <v>0</v>
@@ -2268,10 +2365,10 @@
         <v>0</v>
       </c>
       <c r="N9" s="3">
-        <v>609</v>
+        <v>564</v>
       </c>
       <c r="O9" s="3">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P9" s="3">
         <v>0</v>
@@ -2312,10 +2409,10 @@
         <v>25</v>
       </c>
       <c r="F10" s="3">
-        <v>93</v>
-      </c>
-      <c r="G10" s="7">
-        <v>7.75</v>
+        <v>85</v>
+      </c>
+      <c r="G10" s="6">
+        <v>7.0833333</v>
       </c>
       <c r="H10" s="3">
         <v>12</v>
@@ -2336,10 +2433,10 @@
         <v>0</v>
       </c>
       <c r="N10" s="3">
-        <v>516</v>
+        <v>438</v>
       </c>
       <c r="O10" s="3">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="P10" s="3">
         <v>0</v>
@@ -2374,16 +2471,16 @@
         <v>51</v>
       </c>
       <c r="D11" t="s" s="2">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="E11" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F11" s="3">
-        <v>93</v>
-      </c>
-      <c r="G11" s="7">
-        <v>7.75</v>
+        <v>80</v>
+      </c>
+      <c r="G11" s="6">
+        <v>6.6666666</v>
       </c>
       <c r="H11" s="3">
         <v>12</v>
@@ -2395,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L11" s="3">
         <v>0</v>
@@ -2404,10 +2501,10 @@
         <v>0</v>
       </c>
       <c r="N11" s="3">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="O11" s="3">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="P11" s="3">
         <v>0</v>
@@ -2436,22 +2533,22 @@
         <v>11</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s" s="2">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F12" s="3">
-        <v>93</v>
-      </c>
-      <c r="G12" s="7">
-        <v>7.75</v>
+        <v>79</v>
+      </c>
+      <c r="G12" s="6">
+        <v>6.5833333</v>
       </c>
       <c r="H12" s="3">
         <v>12</v>
@@ -2463,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L12" s="3">
         <v>0</v>
@@ -2472,10 +2569,10 @@
         <v>0</v>
       </c>
       <c r="N12" s="3">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="O12" s="3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="P12" s="3">
         <v>0</v>
@@ -2504,22 +2601,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s" s="2">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F13" s="3">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G13" s="4">
-        <v>7.6666666</v>
+        <v>6.5</v>
       </c>
       <c r="H13" s="3">
         <v>12</v>
@@ -2540,10 +2637,10 @@
         <v>0</v>
       </c>
       <c r="N13" s="3">
-        <v>622</v>
+        <v>480</v>
       </c>
       <c r="O13" s="3">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="P13" s="3">
         <v>0</v>
@@ -2572,22 +2669,22 @@
         <v>13</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s" s="2">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E14" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F14" s="3">
-        <v>91</v>
-      </c>
-      <c r="G14" s="4">
-        <v>7.5833333</v>
+        <v>77</v>
+      </c>
+      <c r="G14" s="6">
+        <v>6.4166666</v>
       </c>
       <c r="H14" s="3">
         <v>12</v>
@@ -2599,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="K14" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L14" s="3">
         <v>0</v>
@@ -2608,10 +2705,10 @@
         <v>0</v>
       </c>
       <c r="N14" s="3">
-        <v>492</v>
+        <v>472</v>
       </c>
       <c r="O14" s="3">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="P14" s="3">
         <v>0</v>
@@ -2640,22 +2737,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F15" s="3">
-        <v>91</v>
-      </c>
-      <c r="G15" s="4">
-        <v>7.5833333</v>
+        <v>76</v>
+      </c>
+      <c r="G15" s="6">
+        <v>6.3333333</v>
       </c>
       <c r="H15" s="3">
         <v>12</v>
@@ -2667,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L15" s="3">
         <v>0</v>
@@ -2676,10 +2773,10 @@
         <v>0</v>
       </c>
       <c r="N15" s="3">
-        <v>553</v>
+        <v>524</v>
       </c>
       <c r="O15" s="3">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P15" s="3">
         <v>0</v>
@@ -2708,22 +2805,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s" s="2">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F16" s="3">
-        <v>91</v>
-      </c>
-      <c r="G16" s="4">
-        <v>7.5833333</v>
+        <v>76</v>
+      </c>
+      <c r="G16" s="6">
+        <v>6.3333333</v>
       </c>
       <c r="H16" s="3">
         <v>12</v>
@@ -2735,19 +2832,19 @@
         <v>0</v>
       </c>
       <c r="K16" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L16" s="3">
         <v>0</v>
       </c>
       <c r="M16" s="3">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="N16" s="3">
-        <v>556</v>
+        <v>477</v>
       </c>
       <c r="O16" s="3">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="P16" s="3">
         <v>0</v>
@@ -2776,22 +2873,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D17" t="s" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E17" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F17" s="3">
-        <v>88</v>
-      </c>
-      <c r="G17" s="4">
-        <v>7.3333333</v>
+        <v>75</v>
+      </c>
+      <c r="G17" s="7">
+        <v>6.25</v>
       </c>
       <c r="H17" s="3">
         <v>12</v>
@@ -2812,10 +2909,10 @@
         <v>0</v>
       </c>
       <c r="N17" s="3">
-        <v>646</v>
+        <v>513</v>
       </c>
       <c r="O17" s="3">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="P17" s="3">
         <v>0</v>
@@ -2844,22 +2941,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s" s="2">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D18" t="s" s="2">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F18" s="3">
-        <v>83</v>
-      </c>
-      <c r="G18" s="4">
-        <v>6.9166666</v>
+        <v>74</v>
+      </c>
+      <c r="G18" s="6">
+        <v>6.1666666</v>
       </c>
       <c r="H18" s="3">
         <v>12</v>
@@ -2880,10 +2977,10 @@
         <v>0</v>
       </c>
       <c r="N18" s="3">
-        <v>598</v>
+        <v>506</v>
       </c>
       <c r="O18" s="3">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="P18" s="3">
         <v>0</v>
@@ -2912,22 +3009,22 @@
         <v>18</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" t="s" s="2">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F19" s="3">
-        <v>81</v>
-      </c>
-      <c r="G19" s="7">
-        <v>6.75</v>
+        <v>70</v>
+      </c>
+      <c r="G19" s="6">
+        <v>5.8333333</v>
       </c>
       <c r="H19" s="3">
         <v>12</v>
@@ -2948,10 +3045,10 @@
         <v>0</v>
       </c>
       <c r="N19" s="3">
-        <v>513</v>
+        <v>405</v>
       </c>
       <c r="O19" s="3">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P19" s="3">
         <v>0</v>
@@ -2980,22 +3077,22 @@
         <v>19</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s" s="2">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E20" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F20" s="3">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G20" s="7">
-        <v>6.75</v>
+        <v>5.75</v>
       </c>
       <c r="H20" s="3">
         <v>12</v>
@@ -3016,10 +3113,10 @@
         <v>0</v>
       </c>
       <c r="N20" s="3">
-        <v>511</v>
+        <v>396</v>
       </c>
       <c r="O20" s="3">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="P20" s="3">
         <v>0</v>
@@ -3048,22 +3145,22 @@
         <v>20</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C21" t="s" s="2">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D21" t="s" s="2">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F21" s="3">
-        <v>80</v>
-      </c>
-      <c r="G21" s="4">
-        <v>6.6666666</v>
+        <v>67</v>
+      </c>
+      <c r="G21" s="6">
+        <v>5.5833333</v>
       </c>
       <c r="H21" s="3">
         <v>12</v>
@@ -3084,10 +3181,10 @@
         <v>0</v>
       </c>
       <c r="N21" s="3">
-        <v>507</v>
+        <v>371</v>
       </c>
       <c r="O21" s="3">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="P21" s="3">
         <v>0</v>
@@ -3116,22 +3213,22 @@
         <v>21</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D22" t="s" s="2">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F22" s="3">
-        <v>78</v>
-      </c>
-      <c r="G22" s="6">
-        <v>6.5</v>
+        <v>66</v>
+      </c>
+      <c r="G22" s="4">
+        <v>5.5</v>
       </c>
       <c r="H22" s="3">
         <v>12</v>
@@ -3152,10 +3249,10 @@
         <v>0</v>
       </c>
       <c r="N22" s="3">
-        <v>489</v>
+        <v>366</v>
       </c>
       <c r="O22" s="3">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="P22" s="3">
         <v>0</v>
@@ -3184,22 +3281,22 @@
         <v>22</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s" s="2">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E23" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F23" s="3">
-        <v>78</v>
-      </c>
-      <c r="G23" s="6">
-        <v>6.5</v>
+        <v>66</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5.5</v>
       </c>
       <c r="H23" s="3">
         <v>12</v>
@@ -3211,7 +3308,7 @@
         <v>0</v>
       </c>
       <c r="K23" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L23" s="3">
         <v>0</v>
@@ -3220,10 +3317,10 @@
         <v>0</v>
       </c>
       <c r="N23" s="3">
-        <v>481</v>
+        <v>425</v>
       </c>
       <c r="O23" s="3">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="P23" s="3">
         <v>0</v>
@@ -3252,22 +3349,22 @@
         <v>23</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C24" t="s" s="2">
         <v>89</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="E24" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F24" s="3">
-        <v>75</v>
-      </c>
-      <c r="G24" s="7">
-        <v>6.25</v>
+        <v>64</v>
+      </c>
+      <c r="G24" s="6">
+        <v>5.3333333</v>
       </c>
       <c r="H24" s="3">
         <v>12</v>
@@ -3288,10 +3385,10 @@
         <v>0</v>
       </c>
       <c r="N24" s="3">
-        <v>451</v>
+        <v>342</v>
       </c>
       <c r="O24" s="3">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="P24" s="3">
         <v>0</v>
@@ -3320,25 +3417,25 @@
         <v>24</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" t="s" s="2">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>49</v>
+        <v>93</v>
       </c>
       <c r="E25" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F25" s="3">
-        <v>65</v>
-      </c>
-      <c r="G25" s="4">
-        <v>5.4166666</v>
+        <v>32</v>
+      </c>
+      <c r="G25" s="6">
+        <v>5.3333333</v>
       </c>
       <c r="H25" s="3">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="I25" s="3">
         <v>0</v>
@@ -3347,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L25" s="3">
         <v>0</v>
@@ -3356,10 +3453,10 @@
         <v>0</v>
       </c>
       <c r="N25" s="3">
-        <v>414</v>
+        <v>203</v>
       </c>
       <c r="O25" s="3">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="P25" s="3">
         <v>0</v>
@@ -3388,22 +3485,22 @@
         <v>25</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C26" t="s" s="2">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D26" t="s" s="2">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E26" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F26" s="3">
-        <v>35</v>
-      </c>
-      <c r="G26" s="4">
-        <v>2.9166666</v>
+        <v>62</v>
+      </c>
+      <c r="G26" s="6">
+        <v>5.1666666</v>
       </c>
       <c r="H26" s="3">
         <v>12</v>
@@ -3415,19 +3512,19 @@
         <v>0</v>
       </c>
       <c r="K26" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L26" s="3">
         <v>0</v>
       </c>
       <c r="M26" s="3">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="N26" s="3">
-        <v>210</v>
+        <v>440</v>
       </c>
       <c r="O26" s="3">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="P26" s="3">
         <v>0</v>
@@ -3456,25 +3553,25 @@
         <v>26</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C27" t="s" s="2">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D27" t="s" s="2">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E27" t="s" s="2">
         <v>25</v>
       </c>
       <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="3">
-        <v>0</v>
+        <v>59</v>
+      </c>
+      <c r="G27" s="6">
+        <v>4.9166666</v>
       </c>
       <c r="H27" s="3">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
@@ -3483,7 +3580,7 @@
         <v>0</v>
       </c>
       <c r="K27" s="3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L27" s="3">
         <v>0</v>
@@ -3492,10 +3589,10 @@
         <v>0</v>
       </c>
       <c r="N27" s="3">
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="O27" s="3">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="P27" s="3">
         <v>0</v>
@@ -3516,6 +3613,822 @@
         <v>0</v>
       </c>
       <c r="V27" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" ht="17" customHeight="1">
+      <c r="A28" s="3">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="D28" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="E28" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F28" s="3">
+        <v>52</v>
+      </c>
+      <c r="G28" s="6">
+        <v>4.3333333</v>
+      </c>
+      <c r="H28" s="3">
+        <v>12</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0</v>
+      </c>
+      <c r="J28" s="3">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3">
+        <v>4</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0</v>
+      </c>
+      <c r="N28" s="3">
+        <v>289</v>
+      </c>
+      <c r="O28" s="3">
+        <v>22</v>
+      </c>
+      <c r="P28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+      <c r="S28" s="5">
+        <v>0</v>
+      </c>
+      <c r="T28" s="3">
+        <v>0</v>
+      </c>
+      <c r="U28" s="3">
+        <v>0</v>
+      </c>
+      <c r="V28" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" ht="17" customHeight="1">
+      <c r="A29" s="3">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s" s="2">
+        <v>103</v>
+      </c>
+      <c r="C29" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s" s="2">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F29" s="3">
+        <v>51</v>
+      </c>
+      <c r="G29" s="7">
+        <v>4.25</v>
+      </c>
+      <c r="H29" s="3">
+        <v>12</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>0</v>
+      </c>
+      <c r="K29" s="3">
+        <v>3</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0</v>
+      </c>
+      <c r="N29" s="3">
+        <v>331</v>
+      </c>
+      <c r="O29" s="3">
+        <v>26</v>
+      </c>
+      <c r="P29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0</v>
+      </c>
+      <c r="R29" s="3">
+        <v>0</v>
+      </c>
+      <c r="S29" s="5">
+        <v>0</v>
+      </c>
+      <c r="T29" s="3">
+        <v>0</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0</v>
+      </c>
+      <c r="V29" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" ht="17" customHeight="1">
+      <c r="A30" s="3">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="D30" t="s" s="2">
+        <v>107</v>
+      </c>
+      <c r="E30" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F30" s="3">
+        <v>49</v>
+      </c>
+      <c r="G30" s="6">
+        <v>4.0833333</v>
+      </c>
+      <c r="H30" s="3">
+        <v>12</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>0</v>
+      </c>
+      <c r="K30" s="3">
+        <v>4</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0</v>
+      </c>
+      <c r="N30" s="3">
+        <v>259</v>
+      </c>
+      <c r="O30" s="3">
+        <v>20</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0</v>
+      </c>
+      <c r="R30" s="3">
+        <v>0</v>
+      </c>
+      <c r="S30" s="5">
+        <v>0</v>
+      </c>
+      <c r="T30" s="3">
+        <v>0</v>
+      </c>
+      <c r="U30" s="3">
+        <v>0</v>
+      </c>
+      <c r="V30" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" ht="17" customHeight="1">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="E31" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F31" s="3">
+        <v>48</v>
+      </c>
+      <c r="G31" s="3">
+        <v>4</v>
+      </c>
+      <c r="H31" s="3">
+        <v>12</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0</v>
+      </c>
+      <c r="J31" s="3">
+        <v>0</v>
+      </c>
+      <c r="K31" s="3">
+        <v>3</v>
+      </c>
+      <c r="L31" s="3">
+        <v>0</v>
+      </c>
+      <c r="M31" s="3">
+        <v>0</v>
+      </c>
+      <c r="N31" s="3">
+        <v>308</v>
+      </c>
+      <c r="O31" s="3">
+        <v>25</v>
+      </c>
+      <c r="P31" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0</v>
+      </c>
+      <c r="R31" s="3">
+        <v>0</v>
+      </c>
+      <c r="S31" s="5">
+        <v>0</v>
+      </c>
+      <c r="T31" s="3">
+        <v>0</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0</v>
+      </c>
+      <c r="V31" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" ht="17" customHeight="1">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="C32" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="E32" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F32" s="3">
+        <v>36</v>
+      </c>
+      <c r="G32" s="4">
+        <v>3.6</v>
+      </c>
+      <c r="H32" s="3">
+        <v>10</v>
+      </c>
+      <c r="I32" s="3">
+        <v>0</v>
+      </c>
+      <c r="J32" s="3">
+        <v>0</v>
+      </c>
+      <c r="K32" s="3">
+        <v>2</v>
+      </c>
+      <c r="L32" s="3">
+        <v>0</v>
+      </c>
+      <c r="M32" s="3">
+        <v>0</v>
+      </c>
+      <c r="N32" s="3">
+        <v>243</v>
+      </c>
+      <c r="O32" s="3">
+        <v>18</v>
+      </c>
+      <c r="P32" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0</v>
+      </c>
+      <c r="R32" s="3">
+        <v>0</v>
+      </c>
+      <c r="S32" s="5">
+        <v>0</v>
+      </c>
+      <c r="T32" s="3">
+        <v>0</v>
+      </c>
+      <c r="U32" s="3">
+        <v>0</v>
+      </c>
+      <c r="V32" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" ht="17" customHeight="1">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s" s="2">
+        <v>113</v>
+      </c>
+      <c r="C33" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D33" t="s" s="2">
+        <v>112</v>
+      </c>
+      <c r="E33" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F33" s="3">
+        <v>37</v>
+      </c>
+      <c r="G33" s="6">
+        <v>3.0833333</v>
+      </c>
+      <c r="H33" s="3">
+        <v>12</v>
+      </c>
+      <c r="I33" s="3">
+        <v>0</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="3">
+        <v>2</v>
+      </c>
+      <c r="L33" s="3">
+        <v>0</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="3">
+        <v>254</v>
+      </c>
+      <c r="O33" s="3">
+        <v>24</v>
+      </c>
+      <c r="P33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>0</v>
+      </c>
+      <c r="R33" s="3">
+        <v>0</v>
+      </c>
+      <c r="S33" s="5">
+        <v>0</v>
+      </c>
+      <c r="T33" s="3">
+        <v>0</v>
+      </c>
+      <c r="U33" s="3">
+        <v>0</v>
+      </c>
+      <c r="V33" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" ht="17" customHeight="1">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>115</v>
+      </c>
+      <c r="D34" t="s" s="2">
+        <v>116</v>
+      </c>
+      <c r="E34" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F34" s="3">
+        <v>36</v>
+      </c>
+      <c r="G34" s="3">
+        <v>3</v>
+      </c>
+      <c r="H34" s="3">
+        <v>12</v>
+      </c>
+      <c r="I34" s="3">
+        <v>0</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="3">
+        <v>2</v>
+      </c>
+      <c r="L34" s="3">
+        <v>0</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="3">
+        <v>244</v>
+      </c>
+      <c r="O34" s="3">
+        <v>14</v>
+      </c>
+      <c r="P34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="5">
+        <v>0</v>
+      </c>
+      <c r="T34" s="3">
+        <v>0</v>
+      </c>
+      <c r="U34" s="3">
+        <v>0</v>
+      </c>
+      <c r="V34" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" ht="17" customHeight="1">
+      <c r="A35" s="3">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s" s="2">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>118</v>
+      </c>
+      <c r="D35" t="s" s="2">
+        <v>119</v>
+      </c>
+      <c r="E35" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F35" s="3">
+        <v>27</v>
+      </c>
+      <c r="G35" s="7">
+        <v>2.25</v>
+      </c>
+      <c r="H35" s="3">
+        <v>12</v>
+      </c>
+      <c r="I35" s="3">
+        <v>0</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="3">
+        <v>1</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="3">
+        <v>214</v>
+      </c>
+      <c r="O35" s="3">
+        <v>15</v>
+      </c>
+      <c r="P35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>0</v>
+      </c>
+      <c r="R35" s="3">
+        <v>0</v>
+      </c>
+      <c r="S35" s="5">
+        <v>0</v>
+      </c>
+      <c r="T35" s="3">
+        <v>0</v>
+      </c>
+      <c r="U35" s="3">
+        <v>0</v>
+      </c>
+      <c r="V35" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" ht="17" customHeight="1">
+      <c r="A36" s="3">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="C36" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="D36" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="E36" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F36" s="3">
+        <v>0</v>
+      </c>
+      <c r="G36" s="3">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>0</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3">
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>0</v>
+      </c>
+      <c r="R36" s="3">
+        <v>0</v>
+      </c>
+      <c r="S36" s="5">
+        <v>0</v>
+      </c>
+      <c r="T36" s="3">
+        <v>0</v>
+      </c>
+      <c r="U36" s="3">
+        <v>0</v>
+      </c>
+      <c r="V36" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" ht="17" customHeight="1">
+      <c r="A37" s="3">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="C37" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="D37" t="s" s="2">
+        <v>125</v>
+      </c>
+      <c r="E37" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>0</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3">
+        <v>0</v>
+      </c>
+      <c r="O37" s="3">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>0</v>
+      </c>
+      <c r="R37" s="3">
+        <v>0</v>
+      </c>
+      <c r="S37" s="5">
+        <v>0</v>
+      </c>
+      <c r="T37" s="3">
+        <v>0</v>
+      </c>
+      <c r="U37" s="3">
+        <v>0</v>
+      </c>
+      <c r="V37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" ht="17" customHeight="1">
+      <c r="A38" s="3">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="C38" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="D38" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="E38" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F38" s="3">
+        <v>0</v>
+      </c>
+      <c r="G38" s="3">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>0</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>0</v>
+      </c>
+      <c r="R38" s="3">
+        <v>0</v>
+      </c>
+      <c r="S38" s="5">
+        <v>0</v>
+      </c>
+      <c r="T38" s="3">
+        <v>0</v>
+      </c>
+      <c r="U38" s="3">
+        <v>0</v>
+      </c>
+      <c r="V38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" ht="17" customHeight="1">
+      <c r="A39" s="3">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="C39" t="s" s="2">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s" s="2">
+        <v>130</v>
+      </c>
+      <c r="E39" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="F39" s="3">
+        <v>0</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="3">
+        <v>0</v>
+      </c>
+      <c r="J39" s="3">
+        <v>0</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0</v>
+      </c>
+      <c r="M39" s="3">
+        <v>0</v>
+      </c>
+      <c r="N39" s="3">
+        <v>0</v>
+      </c>
+      <c r="O39" s="3">
+        <v>0</v>
+      </c>
+      <c r="P39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>0</v>
+      </c>
+      <c r="R39" s="3">
+        <v>0</v>
+      </c>
+      <c r="S39" s="5">
+        <v>0</v>
+      </c>
+      <c r="T39" s="3">
+        <v>0</v>
+      </c>
+      <c r="U39" s="3">
+        <v>0</v>
+      </c>
+      <c r="V39" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>